<commit_message>
feat(volume): add endpoints for retrieving most ordered and low stock volumes
</commit_message>
<xml_diff>
--- a/orders.xlsx
+++ b/orders.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="27">
   <si>
     <t>User Name</t>
   </si>
@@ -71,6 +71,27 @@
   </si>
   <si>
     <t>2025-07-30T11:55:35.754Z</t>
+  </si>
+  <si>
+    <t>assa</t>
+  </si>
+  <si>
+    <t>43215665454765</t>
+  </si>
+  <si>
+    <t>2025-07-31T16:43:59.649Z</t>
+  </si>
+  <si>
+    <t>Sakamoto Days</t>
+  </si>
+  <si>
+    <t>vxbvnb</t>
+  </si>
+  <si>
+    <t>435436465565</t>
+  </si>
+  <si>
+    <t>2025-07-31T16:44:54.370Z</t>
   </si>
 </sst>
 </file>
@@ -447,7 +468,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:K20"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -730,6 +751,426 @@
         <v>189</v>
       </c>
     </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G9">
+        <v>10</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <v>118.8</v>
+      </c>
+      <c r="J9">
+        <v>118.8</v>
+      </c>
+      <c r="K9">
+        <v>1401.3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" t="s">
+        <v>23</v>
+      </c>
+      <c r="G10">
+        <v>6</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <v>118.8</v>
+      </c>
+      <c r="J10">
+        <v>118.8</v>
+      </c>
+      <c r="K10">
+        <v>1401.3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G11">
+        <v>5</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <v>118.8</v>
+      </c>
+      <c r="J11">
+        <v>118.8</v>
+      </c>
+      <c r="K11">
+        <v>1401.3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" t="s">
+        <v>22</v>
+      </c>
+      <c r="F12" t="s">
+        <v>23</v>
+      </c>
+      <c r="G12">
+        <v>4</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="I12">
+        <v>118.8</v>
+      </c>
+      <c r="J12">
+        <v>118.8</v>
+      </c>
+      <c r="K12">
+        <v>1401.3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" t="s">
+        <v>22</v>
+      </c>
+      <c r="F13" t="s">
+        <v>23</v>
+      </c>
+      <c r="G13">
+        <v>3</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="I13">
+        <v>118.8</v>
+      </c>
+      <c r="J13">
+        <v>118.8</v>
+      </c>
+      <c r="K13">
+        <v>1401.3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" t="s">
+        <v>22</v>
+      </c>
+      <c r="F14" t="s">
+        <v>23</v>
+      </c>
+      <c r="G14">
+        <v>2</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="I14">
+        <v>118.8</v>
+      </c>
+      <c r="J14">
+        <v>118.8</v>
+      </c>
+      <c r="K14">
+        <v>1401.3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" t="s">
+        <v>14</v>
+      </c>
+      <c r="E15" t="s">
+        <v>22</v>
+      </c>
+      <c r="F15" t="s">
+        <v>23</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
+      <c r="I15">
+        <v>118.8</v>
+      </c>
+      <c r="J15">
+        <v>118.8</v>
+      </c>
+      <c r="K15">
+        <v>1401.3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" t="s">
+        <v>14</v>
+      </c>
+      <c r="E16" t="s">
+        <v>22</v>
+      </c>
+      <c r="F16" t="s">
+        <v>23</v>
+      </c>
+      <c r="G16">
+        <v>9</v>
+      </c>
+      <c r="H16">
+        <v>1</v>
+      </c>
+      <c r="I16">
+        <v>118.8</v>
+      </c>
+      <c r="J16">
+        <v>118.8</v>
+      </c>
+      <c r="K16">
+        <v>1401.3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" t="s">
+        <v>14</v>
+      </c>
+      <c r="E17" t="s">
+        <v>22</v>
+      </c>
+      <c r="F17" t="s">
+        <v>23</v>
+      </c>
+      <c r="G17">
+        <v>8</v>
+      </c>
+      <c r="H17">
+        <v>2</v>
+      </c>
+      <c r="I17">
+        <v>118.8</v>
+      </c>
+      <c r="J17">
+        <v>237.6</v>
+      </c>
+      <c r="K17">
+        <v>1401.3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" t="s">
+        <v>14</v>
+      </c>
+      <c r="E18" t="s">
+        <v>22</v>
+      </c>
+      <c r="F18" t="s">
+        <v>23</v>
+      </c>
+      <c r="G18">
+        <v>7</v>
+      </c>
+      <c r="H18">
+        <v>1</v>
+      </c>
+      <c r="I18">
+        <v>118.8</v>
+      </c>
+      <c r="J18">
+        <v>118.8</v>
+      </c>
+      <c r="K18">
+        <v>1401.3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" t="s">
+        <v>14</v>
+      </c>
+      <c r="E19" t="s">
+        <v>22</v>
+      </c>
+      <c r="F19" t="s">
+        <v>16</v>
+      </c>
+      <c r="G19">
+        <v>5</v>
+      </c>
+      <c r="H19">
+        <v>1</v>
+      </c>
+      <c r="I19">
+        <v>94.5</v>
+      </c>
+      <c r="J19">
+        <v>94.5</v>
+      </c>
+      <c r="K19">
+        <v>1401.3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20" t="s">
+        <v>14</v>
+      </c>
+      <c r="E20" t="s">
+        <v>26</v>
+      </c>
+      <c r="F20" t="s">
+        <v>23</v>
+      </c>
+      <c r="G20">
+        <v>8</v>
+      </c>
+      <c r="H20">
+        <v>8</v>
+      </c>
+      <c r="I20">
+        <v>118.8</v>
+      </c>
+      <c r="J20">
+        <v>950.4</v>
+      </c>
+      <c r="K20">
+        <v>950.4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>

</xml_diff>

<commit_message>
refactor: remove console log statements from manga, volume, and wishlist services
</commit_message>
<xml_diff>
--- a/orders.xlsx
+++ b/orders.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="36">
   <si>
     <t>User Name</t>
   </si>
@@ -92,6 +92,33 @@
   </si>
   <si>
     <t>2025-07-31T16:44:54.370Z</t>
+  </si>
+  <si>
+    <t>JohnDoe</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>07893830932</t>
+  </si>
+  <si>
+    <t>2025-08-02T12:03:50.585Z</t>
+  </si>
+  <si>
+    <t>Sakamoto days !</t>
+  </si>
+  <si>
+    <t>tanger</t>
+  </si>
+  <si>
+    <t>93932979430</t>
+  </si>
+  <si>
+    <t>2025-08-02T12:04:59.577Z</t>
+  </si>
+  <si>
+    <t>One Piece</t>
   </si>
 </sst>
 </file>
@@ -468,7 +495,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K20"/>
+  <dimension ref="A1:K24"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -1171,6 +1198,146 @@
         <v>950.4</v>
       </c>
     </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21" t="s">
+        <v>29</v>
+      </c>
+      <c r="D21" t="s">
+        <v>14</v>
+      </c>
+      <c r="E21" t="s">
+        <v>30</v>
+      </c>
+      <c r="F21" t="s">
+        <v>31</v>
+      </c>
+      <c r="G21">
+        <v>3</v>
+      </c>
+      <c r="H21">
+        <v>1</v>
+      </c>
+      <c r="I21">
+        <v>108.9</v>
+      </c>
+      <c r="J21">
+        <v>108.9</v>
+      </c>
+      <c r="K21">
+        <v>326.7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" t="s">
+        <v>28</v>
+      </c>
+      <c r="C22" t="s">
+        <v>29</v>
+      </c>
+      <c r="D22" t="s">
+        <v>14</v>
+      </c>
+      <c r="E22" t="s">
+        <v>30</v>
+      </c>
+      <c r="F22" t="s">
+        <v>31</v>
+      </c>
+      <c r="G22">
+        <v>6</v>
+      </c>
+      <c r="H22">
+        <v>2</v>
+      </c>
+      <c r="I22">
+        <v>108.9</v>
+      </c>
+      <c r="J22">
+        <v>217.8</v>
+      </c>
+      <c r="K22">
+        <v>326.7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23" t="s">
+        <v>32</v>
+      </c>
+      <c r="C23" t="s">
+        <v>33</v>
+      </c>
+      <c r="D23" t="s">
+        <v>14</v>
+      </c>
+      <c r="E23" t="s">
+        <v>34</v>
+      </c>
+      <c r="F23" t="s">
+        <v>35</v>
+      </c>
+      <c r="G23">
+        <v>4</v>
+      </c>
+      <c r="H23">
+        <v>42</v>
+      </c>
+      <c r="I23">
+        <v>108.9</v>
+      </c>
+      <c r="J23">
+        <v>4573.8</v>
+      </c>
+      <c r="K23">
+        <v>9365.4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" t="s">
+        <v>32</v>
+      </c>
+      <c r="C24" t="s">
+        <v>33</v>
+      </c>
+      <c r="D24" t="s">
+        <v>14</v>
+      </c>
+      <c r="E24" t="s">
+        <v>34</v>
+      </c>
+      <c r="F24" t="s">
+        <v>31</v>
+      </c>
+      <c r="G24">
+        <v>2</v>
+      </c>
+      <c r="H24">
+        <v>44</v>
+      </c>
+      <c r="I24">
+        <v>108.9</v>
+      </c>
+      <c r="J24">
+        <v>4791.6</v>
+      </c>
+      <c r="K24">
+        <v>9365.4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>

</xml_diff>